<commit_message>
25 1421 sprint 2 -- chemin optimal
</commit_message>
<xml_diff>
--- a/sprint_backlog.xlsx
+++ b/sprint_backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
   <si>
     <t>N°</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>afficher l'état du traffic(perturbations du réseau,temps d'arrêt)</t>
+  </si>
+  <si>
+    <t>trouver les chemins les plus courts pour arriver à chaque station</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1127,7 @@
           <c:x val="0.11197945144513816"/>
           <c:y val="0.125"/>
           <c:w val="0.8385437991938256"/>
-          <c:h val="0.66500000000000148"/>
+          <c:h val="0.6650000000000017"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1298,8 +1301,8 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="50"/>
-        <c:axId val="60608512"/>
-        <c:axId val="63255296"/>
+        <c:axId val="61831424"/>
+        <c:axId val="61841408"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1644,11 +1647,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="60608512"/>
-        <c:axId val="63255296"/>
+        <c:axId val="61831424"/>
+        <c:axId val="61841408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60608512"/>
+        <c:axId val="61831424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1672,14 +1675,14 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63255296"/>
+        <c:crossAx val="61841408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63255296"/>
+        <c:axId val="61841408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -1715,7 +1718,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60608512"/>
+        <c:crossAx val="61831424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1728,8 +1731,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.62500158946123618"/>
           <c:y val="2.5000000000000001E-2"/>
-          <c:w val="0.27512166447944048"/>
-          <c:h val="0.26462572178477717"/>
+          <c:w val="0.27512166447944053"/>
+          <c:h val="0.26462572178477722"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1791,7 +1794,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3050,8 +3053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:AK60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3449,11 +3452,11 @@
       <c r="G22" s="2"/>
       <c r="H22" s="48">
         <f>SUM(H23:H35,H14:H21)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I22" s="48">
         <f>SUM(I23:I46,I14:I21)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -3587,13 +3590,21 @@
     </row>
     <row r="27" spans="2:37">
       <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
+      <c r="C27" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>40</v>
+      </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="H27" s="1">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1">
+        <v>2</v>
+      </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>

</xml_diff>

<commit_message>
25 1421 sprint 2 -- recherche
</commit_message>
<xml_diff>
--- a/sprint_backlog.xlsx
+++ b/sprint_backlog.xlsx
@@ -13,7 +13,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="log_member_names">'[1]Timesheet Template - Log type'!$C$4:$C$328</definedName>
@@ -21,11 +20,12 @@
     <definedName name="team_members">[1]Legend!$D$3:$D$9</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
   <si>
     <t>N°</t>
   </si>
@@ -238,6 +238,33 @@
   </si>
   <si>
     <t>trouver les chemins les plus courts pour arriver à chaque station</t>
+  </si>
+  <si>
+    <t>trouver le trajet avec le moins de changements de lignes</t>
+  </si>
+  <si>
+    <t>interface utilisateur</t>
+  </si>
+  <si>
+    <t>Histoire</t>
+  </si>
+  <si>
+    <t>à faire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>tests à faire</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>créer le réseau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">architecture </t>
   </si>
 </sst>
 </file>
@@ -402,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -634,11 +661,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -734,6 +787,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1127,7 +1182,7 @@
           <c:x val="0.11197945144513816"/>
           <c:y val="0.125"/>
           <c:w val="0.8385437991938256"/>
-          <c:h val="0.6650000000000017"/>
+          <c:h val="0.66500000000000203"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1136,17 +1191,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'[2]Burndown Chart'!$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Daily Completed</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="808080"/>
@@ -1155,154 +1199,19 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'[2]Burndown Chart'!$B$5:$B$25</c:f>
+              <c:f>Feuil1!$K$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[2]Burndown Chart'!$G$5:$G$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>#N/A</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:gapWidth val="50"/>
-        <c:axId val="61831424"/>
-        <c:axId val="61841408"/>
+        <c:axId val="59862400"/>
+        <c:axId val="59872384"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1310,15 +1219,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'[2]Burndown Chart'!$E$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Planned</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>planifié</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="38100">
@@ -1331,146 +1232,14 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'[2]Burndown Chart'!$B$5:$B$25</c:f>
+              <c:f>Feuil1!$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[2]Burndown Chart'!$E$5:$E$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>238</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>209</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>194</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>184</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>164</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>126</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>107</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>86</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>74</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1480,15 +1249,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'[2]Burndown Chart'!$F$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Actual</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>réalisé</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="38100">
@@ -1501,157 +1262,25 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>'[2]Burndown Chart'!$B$5:$B$25</c:f>
+              <c:f>Feuil1!$I$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[2]Burndown Chart'!$F$5:$F$25</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>250</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>242</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>232</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>220</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>201</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>188</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>178</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>176</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>140</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>#N/A</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="61831424"/>
-        <c:axId val="61841408"/>
+        <c:axId val="59862400"/>
+        <c:axId val="59872384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61831424"/>
+        <c:axId val="59862400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1675,17 +1304,16 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61841408"/>
+        <c:crossAx val="59872384"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61841408"/>
+        <c:axId val="59872384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="300"/>
+          <c:max val="20"/>
           <c:min val="0"/>
         </c:scaling>
         <c:axPos val="l"/>
@@ -1718,9 +1346,10 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61831424"/>
+        <c:crossAx val="59862400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1731,8 +1360,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.62500158946123618"/>
           <c:y val="2.5000000000000001E-2"/>
-          <c:w val="0.27512166447944053"/>
-          <c:h val="0.26462572178477722"/>
+          <c:w val="0.17057198019351033"/>
+          <c:h val="0.1587754330708662"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1794,8 +1423,97 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="bg-BG"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dLbls>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>sprint1</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$H$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showVal val="1"/>
+        </c:dLbls>
+        <c:gapWidth val="95"/>
+        <c:overlap val="100"/>
+        <c:axId val="59891712"/>
+        <c:axId val="59893248"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="59891712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59893248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="59893248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="59891712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1804,16 +1522,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1829,6 +1547,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2397,330 +2145,9 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Burndown Chart"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="G3" t="str">
-            <v>Daily Completed</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="E4" t="str">
-            <v>Planned</v>
-          </cell>
-          <cell r="F4" t="str">
-            <v>Actual</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>0</v>
-          </cell>
-          <cell r="E5">
-            <v>250</v>
-          </cell>
-          <cell r="F5">
-            <v>250</v>
-          </cell>
-          <cell r="G5" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>1</v>
-          </cell>
-          <cell r="E6">
-            <v>238</v>
-          </cell>
-          <cell r="F6">
-            <v>242</v>
-          </cell>
-          <cell r="G6">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>2</v>
-          </cell>
-          <cell r="E7">
-            <v>220</v>
-          </cell>
-          <cell r="F7">
-            <v>232</v>
-          </cell>
-          <cell r="G7">
-            <v>10</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>3</v>
-          </cell>
-          <cell r="E8">
-            <v>209</v>
-          </cell>
-          <cell r="F8">
-            <v>232</v>
-          </cell>
-          <cell r="G8">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>4</v>
-          </cell>
-          <cell r="E9">
-            <v>205</v>
-          </cell>
-          <cell r="F9">
-            <v>220</v>
-          </cell>
-          <cell r="G9">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>5</v>
-          </cell>
-          <cell r="E10">
-            <v>200</v>
-          </cell>
-          <cell r="F10">
-            <v>201</v>
-          </cell>
-          <cell r="G10">
-            <v>19</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>6</v>
-          </cell>
-          <cell r="E11">
-            <v>194</v>
-          </cell>
-          <cell r="F11">
-            <v>188</v>
-          </cell>
-          <cell r="G11">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>7</v>
-          </cell>
-          <cell r="E12">
-            <v>184</v>
-          </cell>
-          <cell r="F12">
-            <v>180</v>
-          </cell>
-          <cell r="G12">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>8</v>
-          </cell>
-          <cell r="E13">
-            <v>164</v>
-          </cell>
-          <cell r="F13">
-            <v>178</v>
-          </cell>
-          <cell r="G13">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>9</v>
-          </cell>
-          <cell r="E14">
-            <v>144</v>
-          </cell>
-          <cell r="F14" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="G14" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>10</v>
-          </cell>
-          <cell r="E15">
-            <v>126</v>
-          </cell>
-          <cell r="F15">
-            <v>176</v>
-          </cell>
-          <cell r="G15">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>11</v>
-          </cell>
-          <cell r="E16">
-            <v>120</v>
-          </cell>
-          <cell r="F16" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="G16" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>12</v>
-          </cell>
-          <cell r="E17">
-            <v>107</v>
-          </cell>
-          <cell r="F17">
-            <v>174</v>
-          </cell>
-          <cell r="G17">
-            <v>2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>13</v>
-          </cell>
-          <cell r="E18">
-            <v>100</v>
-          </cell>
-          <cell r="F18">
-            <v>140</v>
-          </cell>
-          <cell r="G18">
-            <v>34</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19">
-            <v>14</v>
-          </cell>
-          <cell r="E19">
-            <v>86</v>
-          </cell>
-          <cell r="F19" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="G19" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="B20">
-            <v>15</v>
-          </cell>
-          <cell r="E20">
-            <v>74</v>
-          </cell>
-          <cell r="F20" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="G20" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="B21">
-            <v>16</v>
-          </cell>
-          <cell r="E21">
-            <v>60</v>
-          </cell>
-          <cell r="F21" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="G21" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22">
-            <v>17</v>
-          </cell>
-          <cell r="E22">
-            <v>48</v>
-          </cell>
-          <cell r="F22" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="G22" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23">
-            <v>18</v>
-          </cell>
-          <cell r="E23">
-            <v>37</v>
-          </cell>
-          <cell r="F23" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="G23" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24">
-            <v>19</v>
-          </cell>
-          <cell r="E24">
-            <v>18</v>
-          </cell>
-          <cell r="F24" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="G24" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25">
-            <v>20</v>
-          </cell>
-          <cell r="E25">
-            <v>0</v>
-          </cell>
-          <cell r="F25" t="e">
-            <v>#N/A</v>
-          </cell>
-          <cell r="G25" t="e">
-            <v>#N/A</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B10:O52" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="B10:O52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B10:O53" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="B10:O53">
     <filterColumn colId="4"/>
     <filterColumn colId="6"/>
     <filterColumn colId="7"/>
@@ -2752,8 +2179,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="E54:J60" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="E54:J60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="E55:J61" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="E55:J61"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Colonne1" dataDxfId="5"/>
     <tableColumn id="2" name="Colonne2" dataDxfId="4"/>
@@ -2763,6 +2190,24 @@
     <tableColumn id="6" name="Colonne6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="B4:J36" totalsRowShown="0">
+  <autoFilter ref="B4:J36"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Histoire"/>
+    <tableColumn id="2" name="à faire"/>
+    <tableColumn id="3" name="  "/>
+    <tableColumn id="4" name="en cours"/>
+    <tableColumn id="5" name="     "/>
+    <tableColumn id="6" name="tests à faire"/>
+    <tableColumn id="7" name="    "/>
+    <tableColumn id="8" name="fait"/>
+    <tableColumn id="9" name="   "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3051,10 +2496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:AK60"/>
+  <dimension ref="B3:AK61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3108,7 +2553,7 @@
       </c>
       <c r="E8" s="29">
         <f ca="1">DATEDIF(NOW(),E7,"D")</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -3226,11 +2671,11 @@
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="48">
+      <c r="F13" s="49">
         <f>SUM(F14:F21)</f>
         <v>6</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="50">
         <f>SUM(G14:G21)</f>
         <v>6</v>
       </c>
@@ -3326,7 +2771,7 @@
     </row>
     <row r="17" spans="2:37">
       <c r="B17" s="7">
-        <f t="shared" ref="B17:B21" si="0">SUM(B16,1)</f>
+        <f>SUM(B16,1)</f>
         <v>3</v>
       </c>
       <c r="C17" s="6" t="s">
@@ -3349,7 +2794,7 @@
     </row>
     <row r="18" spans="2:37">
       <c r="B18" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B17,1)</f>
         <v>4</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -3372,7 +2817,7 @@
     </row>
     <row r="19" spans="2:37">
       <c r="B19" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B18,1)</f>
         <v>5</v>
       </c>
       <c r="C19" s="6" t="s">
@@ -3395,7 +2840,7 @@
     </row>
     <row r="20" spans="2:37">
       <c r="B20" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B19,1)</f>
         <v>6</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -3418,7 +2863,7 @@
     </row>
     <row r="21" spans="2:37">
       <c r="B21" s="7">
-        <f t="shared" si="0"/>
+        <f>SUM(B20,1)</f>
         <v>7</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -3439,84 +2884,68 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="2:37" s="36" customFormat="1" ht="18.75">
-      <c r="B22" s="32" t="s">
+    <row r="22" spans="2:37">
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:37" s="36" customFormat="1" ht="18.75">
+      <c r="B23" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C23" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="48">
-        <f>SUM(H23:H35,H14:H21)</f>
+      <c r="D23" s="35"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="49">
+        <f>SUM(H24:H36,H14:H21)</f>
         <v>31</v>
       </c>
-      <c r="I22" s="48">
-        <f>SUM(I23:I46,I14:I21)</f>
-        <v>19</v>
-      </c>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-    </row>
-    <row r="23" spans="2:37" s="37" customFormat="1" ht="18.75">
-      <c r="B23" s="38"/>
-      <c r="C23" s="39" t="s">
+      <c r="I23" s="50">
+        <f>SUM(I24:I47,I14:I21)</f>
+        <v>22</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+    </row>
+    <row r="24" spans="2:37" s="37" customFormat="1" ht="18.75">
+      <c r="B24" s="38"/>
+      <c r="C24" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="41" t="s">
+      <c r="D24" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40">
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40">
         <v>1</v>
       </c>
-      <c r="I23" s="40">
+      <c r="I24" s="40">
         <v>1</v>
       </c>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40"/>
-    </row>
-    <row r="24" spans="2:37" ht="18.75">
-      <c r="B24" s="33"/>
-      <c r="C24" s="34" t="s">
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="40"/>
+      <c r="N24" s="40"/>
+      <c r="O24" s="40"/>
+    </row>
+    <row r="25" spans="2:37" ht="18.75">
+      <c r="B25" s="33"/>
+      <c r="C25" s="34" t="s">
         <v>60</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1">
-        <v>1</v>
-      </c>
-      <c r="G24" s="1">
-        <v>1</v>
-      </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="2:37">
-      <c r="B25" s="7"/>
-      <c r="C25" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D25" s="31" t="s">
         <v>40</v>
@@ -3528,12 +2957,8 @@
       <c r="G25" s="1">
         <v>1</v>
       </c>
-      <c r="H25" s="1">
-        <v>2</v>
-      </c>
-      <c r="I25" s="1">
-        <v>2</v>
-      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -3541,22 +2966,26 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="2:37" ht="23.25">
-      <c r="B26" s="42"/>
-      <c r="C26" s="42" t="s">
-        <v>64</v>
+    <row r="26" spans="2:37">
+      <c r="B26" s="7"/>
+      <c r="C26" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="D26" s="31" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
       <c r="H26" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I26" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -3564,34 +2993,11 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
-      <c r="Q26" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="R26" s="49"/>
-      <c r="S26" s="49"/>
-      <c r="T26" s="49"/>
-      <c r="U26" s="49"/>
-      <c r="V26" s="49"/>
-      <c r="W26" s="49"/>
-      <c r="X26" s="49"/>
-      <c r="Y26" s="49"/>
-      <c r="Z26" s="49"/>
-      <c r="AA26" s="49"/>
-      <c r="AB26" s="49"/>
-      <c r="AC26" s="49"/>
-      <c r="AD26" s="49"/>
-      <c r="AE26" s="49"/>
-      <c r="AF26" s="49"/>
-      <c r="AG26" s="49"/>
-      <c r="AH26" s="49"/>
-      <c r="AI26" s="49"/>
-      <c r="AJ26" s="49"/>
-      <c r="AK26" s="49"/>
-    </row>
-    <row r="27" spans="2:37">
+    </row>
+    <row r="27" spans="2:37" ht="23.25">
       <c r="B27" s="42"/>
       <c r="C27" s="42" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D27" s="31" t="s">
         <v>40</v>
@@ -3600,10 +3006,10 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I27" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -3611,48 +3017,46 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="Q27" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="R27" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
-      <c r="U27" s="53"/>
-      <c r="V27" s="53"/>
-      <c r="W27" s="53"/>
-      <c r="X27" s="53"/>
-      <c r="Y27" s="53"/>
-      <c r="Z27" s="53"/>
-      <c r="AA27" s="53"/>
-      <c r="AB27" s="53"/>
-      <c r="AC27" s="53"/>
-      <c r="AD27" s="53"/>
-      <c r="AE27" s="53"/>
-      <c r="AF27" s="53"/>
-      <c r="AG27" s="53"/>
-      <c r="AH27" s="53"/>
-      <c r="AI27" s="53"/>
-      <c r="AJ27" s="53"/>
-      <c r="AK27" s="54"/>
+      <c r="Q27" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="R27" s="51"/>
+      <c r="S27" s="51"/>
+      <c r="T27" s="51"/>
+      <c r="U27" s="51"/>
+      <c r="V27" s="51"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="51"/>
+      <c r="Y27" s="51"/>
+      <c r="Z27" s="51"/>
+      <c r="AA27" s="51"/>
+      <c r="AB27" s="51"/>
+      <c r="AC27" s="51"/>
+      <c r="AD27" s="51"/>
+      <c r="AE27" s="51"/>
+      <c r="AF27" s="51"/>
+      <c r="AG27" s="51"/>
+      <c r="AH27" s="51"/>
+      <c r="AI27" s="51"/>
+      <c r="AJ27" s="51"/>
+      <c r="AK27" s="51"/>
     </row>
     <row r="28" spans="2:37">
-      <c r="B28" s="43"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="45" t="s">
-        <v>4</v>
+        <v>70</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>40</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I28" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -3660,102 +3064,91 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="9">
-        <v>1</v>
-      </c>
-      <c r="S28" s="9">
-        <v>2</v>
-      </c>
-      <c r="T28" s="9">
-        <v>3</v>
-      </c>
-      <c r="U28" s="9">
-        <v>4</v>
-      </c>
-      <c r="V28" s="9">
-        <v>5</v>
-      </c>
-      <c r="W28" s="9"/>
-      <c r="X28" s="9"/>
-      <c r="Y28" s="9"/>
-      <c r="Z28" s="9"/>
-      <c r="AA28" s="9"/>
-      <c r="AB28" s="9"/>
-      <c r="AC28" s="9"/>
-      <c r="AD28" s="9"/>
-      <c r="AE28" s="9"/>
-      <c r="AF28" s="9"/>
-      <c r="AG28" s="9"/>
-      <c r="AH28" s="9"/>
-      <c r="AI28" s="9"/>
-      <c r="AJ28" s="9"/>
-      <c r="AK28" s="10"/>
+      <c r="Q28" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="R28" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="S28" s="55"/>
+      <c r="T28" s="55"/>
+      <c r="U28" s="55"/>
+      <c r="V28" s="55"/>
+      <c r="W28" s="55"/>
+      <c r="X28" s="55"/>
+      <c r="Y28" s="55"/>
+      <c r="Z28" s="55"/>
+      <c r="AA28" s="55"/>
+      <c r="AB28" s="55"/>
+      <c r="AC28" s="55"/>
+      <c r="AD28" s="55"/>
+      <c r="AE28" s="55"/>
+      <c r="AF28" s="55"/>
+      <c r="AG28" s="55"/>
+      <c r="AH28" s="55"/>
+      <c r="AI28" s="55"/>
+      <c r="AJ28" s="55"/>
+      <c r="AK28" s="56"/>
     </row>
     <row r="29" spans="2:37">
       <c r="B29" s="43"/>
       <c r="C29" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="D29" s="46" t="s">
+        <v>40</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1">
+        <v>6</v>
+      </c>
+      <c r="I29" s="1">
         <v>4</v>
       </c>
-      <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="Q29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R29" s="22">
-        <f t="shared" ref="R29:V31" si="1">SUMPRODUCT(--(log_member_names=$B32),--(log_weeknums=M$5))</f>
-        <v>262</v>
-      </c>
-      <c r="S29" s="23">
-        <f t="shared" si="1"/>
-        <v>262</v>
-      </c>
-      <c r="T29" s="23">
-        <f t="shared" si="1"/>
-        <v>262</v>
-      </c>
-      <c r="U29" s="23">
-        <f t="shared" si="1"/>
-        <v>262</v>
-      </c>
-      <c r="V29" s="23">
-        <f t="shared" si="1"/>
-        <v>262</v>
-      </c>
-      <c r="W29" s="12"/>
-      <c r="X29" s="12"/>
-      <c r="Y29" s="12"/>
-      <c r="Z29" s="12"/>
-      <c r="AA29" s="12"/>
-      <c r="AB29" s="12"/>
-      <c r="AC29" s="12"/>
-      <c r="AD29" s="12"/>
-      <c r="AE29" s="12"/>
-      <c r="AF29" s="12"/>
-      <c r="AG29" s="12"/>
-      <c r="AH29" s="12"/>
-      <c r="AI29" s="12"/>
-      <c r="AJ29" s="12"/>
-      <c r="AK29" s="13"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="9">
+        <v>1</v>
+      </c>
+      <c r="S29" s="9">
+        <v>2</v>
+      </c>
+      <c r="T29" s="9">
+        <v>3</v>
+      </c>
+      <c r="U29" s="9">
+        <v>4</v>
+      </c>
+      <c r="V29" s="9">
+        <v>5</v>
+      </c>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
+      <c r="AB29" s="9"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="9"/>
+      <c r="AI29" s="9"/>
+      <c r="AJ29" s="9"/>
+      <c r="AK29" s="10"/>
     </row>
     <row r="30" spans="2:37">
       <c r="B30" s="43"/>
       <c r="C30" s="42" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="D30" s="44" t="s">
         <v>22</v>
@@ -3764,7 +3157,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
@@ -3773,27 +3166,27 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="Q30" s="17" t="s">
-        <v>14</v>
+      <c r="Q30" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="R30" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="R30:V32" si="0">SUMPRODUCT(--(log_member_names=$B33),--(log_weeknums=M$5))</f>
         <v>262</v>
       </c>
       <c r="S30" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="T30" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="U30" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="V30" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="W30" s="12"/>
@@ -3815,16 +3208,16 @@
     <row r="31" spans="2:37">
       <c r="B31" s="43"/>
       <c r="C31" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="45" t="s">
-        <v>4</v>
+        <v>58</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>22</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
@@ -3833,27 +3226,27 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="Q31" s="18" t="s">
-        <v>15</v>
+      <c r="Q31" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="R31" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="S31" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="T31" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="U31" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="V31" s="23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>262</v>
       </c>
       <c r="W31" s="12"/>
@@ -3875,7 +3268,7 @@
     <row r="32" spans="2:37">
       <c r="B32" s="43"/>
       <c r="C32" s="42" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D32" s="45" t="s">
         <v>4</v>
@@ -3895,26 +3288,28 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
-      <c r="Q32" s="11"/>
+      <c r="Q32" s="18" t="s">
+        <v>15</v>
+      </c>
       <c r="R32" s="22">
-        <f t="shared" ref="R32:V35" si="2">SUMPRODUCT(--(log_member_names=$B16),--(log_weeknums=M$5))</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>262</v>
       </c>
       <c r="S32" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>262</v>
       </c>
       <c r="T32" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>262</v>
       </c>
       <c r="U32" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>262</v>
       </c>
       <c r="V32" s="23">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>262</v>
       </c>
       <c r="W32" s="12"/>
       <c r="X32" s="12"/>
@@ -3935,7 +3330,7 @@
     <row r="33" spans="2:37">
       <c r="B33" s="43"/>
       <c r="C33" s="42" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D33" s="45" t="s">
         <v>4</v>
@@ -3944,10 +3339,10 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -3957,23 +3352,23 @@
       <c r="O33" s="1"/>
       <c r="Q33" s="11"/>
       <c r="R33" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="R33:V36" si="1">SUMPRODUCT(--(log_member_names=$B16),--(log_weeknums=M$5))</f>
         <v>0</v>
       </c>
       <c r="S33" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T33" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U33" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V33" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W33" s="12"/>
@@ -3995,7 +3390,7 @@
     <row r="34" spans="2:37">
       <c r="B34" s="43"/>
       <c r="C34" s="42" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D34" s="46" t="s">
         <v>40</v>
@@ -4017,23 +3412,23 @@
       <c r="O34" s="1"/>
       <c r="Q34" s="11"/>
       <c r="R34" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S34" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="T34" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="U34" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="V34" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W34" s="12"/>
@@ -4055,76 +3450,76 @@
     <row r="35" spans="2:37">
       <c r="B35" s="43"/>
       <c r="C35" s="42" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="D35" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42">
+        <v>40</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1">
         <v>1</v>
       </c>
-      <c r="I35" s="42">
+      <c r="I35" s="1">
         <v>1</v>
       </c>
-      <c r="J35" s="42"/>
+      <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="24">
-        <f t="shared" si="2"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="22">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S35" s="25">
-        <f t="shared" si="2"/>
+      <c r="S35" s="23">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T35" s="25">
-        <f t="shared" si="2"/>
+      <c r="T35" s="23">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U35" s="25">
-        <f t="shared" si="2"/>
+      <c r="U35" s="23">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V35" s="25">
-        <f t="shared" si="2"/>
+      <c r="V35" s="23">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W35" s="15"/>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="15"/>
-      <c r="Z35" s="15"/>
-      <c r="AA35" s="15"/>
-      <c r="AB35" s="15"/>
-      <c r="AC35" s="15"/>
-      <c r="AD35" s="15"/>
-      <c r="AE35" s="15"/>
-      <c r="AF35" s="15"/>
-      <c r="AG35" s="15"/>
-      <c r="AH35" s="15"/>
-      <c r="AI35" s="15"/>
-      <c r="AJ35" s="15"/>
-      <c r="AK35" s="16"/>
+      <c r="W35" s="12"/>
+      <c r="X35" s="12"/>
+      <c r="Y35" s="12"/>
+      <c r="Z35" s="12"/>
+      <c r="AA35" s="12"/>
+      <c r="AB35" s="12"/>
+      <c r="AC35" s="12"/>
+      <c r="AD35" s="12"/>
+      <c r="AE35" s="12"/>
+      <c r="AF35" s="12"/>
+      <c r="AG35" s="12"/>
+      <c r="AH35" s="12"/>
+      <c r="AI35" s="12"/>
+      <c r="AJ35" s="12"/>
+      <c r="AK35" s="13"/>
     </row>
     <row r="36" spans="2:37">
       <c r="B36" s="43"/>
       <c r="C36" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="D36" s="45" t="s">
-        <v>4</v>
+        <v>69</v>
+      </c>
+      <c r="D36" s="46" t="s">
+        <v>67</v>
       </c>
       <c r="E36" s="42"/>
       <c r="F36" s="42"/>
       <c r="G36" s="42"/>
       <c r="H36" s="42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="42">
         <v>1</v>
@@ -4135,71 +3530,116 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S36" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T36" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U36" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V36" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W36" s="15"/>
+      <c r="X36" s="15"/>
+      <c r="Y36" s="15"/>
+      <c r="Z36" s="15"/>
+      <c r="AA36" s="15"/>
+      <c r="AB36" s="15"/>
+      <c r="AC36" s="15"/>
+      <c r="AD36" s="15"/>
+      <c r="AE36" s="15"/>
+      <c r="AF36" s="15"/>
+      <c r="AG36" s="15"/>
+      <c r="AH36" s="15"/>
+      <c r="AI36" s="15"/>
+      <c r="AJ36" s="15"/>
+      <c r="AK36" s="16"/>
     </row>
     <row r="37" spans="2:37">
-      <c r="B37" s="42"/>
+      <c r="B37" s="43"/>
       <c r="C37" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="42"/>
+        <v>28</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>40</v>
+      </c>
       <c r="E37" s="42"/>
       <c r="F37" s="42"/>
       <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
+      <c r="H37" s="42">
+        <v>2</v>
+      </c>
+      <c r="I37" s="42">
+        <v>1</v>
+      </c>
       <c r="J37" s="42"/>
-      <c r="K37" s="42"/>
-      <c r="L37" s="42"/>
-      <c r="M37" s="42"/>
-      <c r="N37" s="42"/>
-      <c r="O37" s="42"/>
-    </row>
-    <row r="39" spans="2:37" s="36" customFormat="1" ht="18.75">
-      <c r="B39" s="32" t="s">
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="2:37">
+      <c r="B38" s="42"/>
+      <c r="C38" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="42"/>
+      <c r="E38" s="42"/>
+      <c r="F38" s="42"/>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="42"/>
+      <c r="L38" s="42"/>
+      <c r="M38" s="42"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="42"/>
+    </row>
+    <row r="39" spans="2:37">
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="2:37" s="36" customFormat="1" ht="18.75">
+      <c r="B40" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="35"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-    </row>
-    <row r="40" spans="2:37">
-      <c r="B40" s="43"/>
-      <c r="C40" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1">
-        <v>3</v>
-      </c>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="48">
+        <v>5</v>
+      </c>
+      <c r="K40" s="48"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
     </row>
     <row r="41" spans="2:37">
       <c r="B41" s="43"/>
       <c r="C41" s="42" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D41" s="44" t="s">
         <v>22</v>
@@ -4221,7 +3661,7 @@
     <row r="42" spans="2:37">
       <c r="B42" s="43"/>
       <c r="C42" s="42" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="D42" s="44" t="s">
         <v>22</v>
@@ -4232,7 +3672,7 @@
       <c r="H42" s="42"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -4241,9 +3681,9 @@
       <c r="O42" s="1"/>
     </row>
     <row r="43" spans="2:37">
-      <c r="B43" s="7"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D43" s="44" t="s">
         <v>22</v>
@@ -4254,7 +3694,7 @@
       <c r="H43" s="42"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -4265,10 +3705,10 @@
     <row r="44" spans="2:37">
       <c r="B44" s="7"/>
       <c r="C44" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="46" t="s">
-        <v>40</v>
+        <v>57</v>
+      </c>
+      <c r="D44" s="44" t="s">
+        <v>22</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -4276,7 +3716,7 @@
       <c r="H44" s="42"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -4285,21 +3725,21 @@
       <c r="O44" s="1"/>
     </row>
     <row r="45" spans="2:37">
-      <c r="B45" s="43"/>
+      <c r="B45" s="7"/>
       <c r="C45" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" s="42"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42">
+        <v>23</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1">
         <v>2</v>
       </c>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -4309,7 +3749,7 @@
     <row r="46" spans="2:37">
       <c r="B46" s="43"/>
       <c r="C46" s="42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D46" s="44" t="s">
         <v>22</v>
@@ -4317,9 +3757,7 @@
       <c r="E46" s="42"/>
       <c r="F46" s="42"/>
       <c r="G46" s="42"/>
-      <c r="H46" s="42">
-        <v>2</v>
-      </c>
+      <c r="H46" s="42"/>
       <c r="I46" s="42"/>
       <c r="J46" s="42"/>
       <c r="K46" s="1"/>
@@ -4329,9 +3767,13 @@
       <c r="O46" s="1"/>
     </row>
     <row r="47" spans="2:37">
-      <c r="B47" s="1"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D47" s="44" t="s">
+        <v>22</v>
+      </c>
       <c r="E47" s="42"/>
       <c r="F47" s="42"/>
       <c r="G47" s="42"/>
@@ -4346,7 +3788,9 @@
     </row>
     <row r="48" spans="2:37">
       <c r="B48" s="1"/>
-      <c r="C48" s="42"/>
+      <c r="C48" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="D48" s="42"/>
       <c r="E48" s="42"/>
       <c r="F48" s="42"/>
@@ -4362,7 +3806,9 @@
     </row>
     <row r="49" spans="2:15">
       <c r="B49" s="1"/>
-      <c r="C49" s="42"/>
+      <c r="C49" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="D49" s="42"/>
       <c r="E49" s="42"/>
       <c r="F49" s="42"/>
@@ -4378,14 +3824,14 @@
     </row>
     <row r="50" spans="2:15">
       <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
+      <c r="J50" s="42"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -4424,36 +3870,44 @@
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
     </row>
-    <row r="54" spans="2:15" hidden="1">
-      <c r="E54" t="s">
+    <row r="53" spans="2:15">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+    </row>
+    <row r="55" spans="2:15" hidden="1">
+      <c r="E55" t="s">
         <v>5</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F55" t="s">
         <v>6</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>7</v>
       </c>
-      <c r="H54" t="s">
+      <c r="H55" t="s">
         <v>8</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I55" t="s">
         <v>9</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J55" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="2:15" ht="15.75">
-      <c r="E55" s="19"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-    </row>
-    <row r="56" spans="2:15">
-      <c r="E56" s="20"/>
+    <row r="56" spans="2:15" ht="15.75">
+      <c r="E56" s="19"/>
       <c r="F56" s="20"/>
       <c r="G56" s="20"/>
       <c r="H56" s="20"/>
@@ -4469,7 +3923,7 @@
       <c r="J57" s="20"/>
     </row>
     <row r="58" spans="2:15">
-      <c r="E58" s="21"/>
+      <c r="E58" s="20"/>
       <c r="F58" s="20"/>
       <c r="G58" s="20"/>
       <c r="H58" s="20"/>
@@ -4492,13 +3946,21 @@
       <c r="I60" s="20"/>
       <c r="J60" s="20"/>
     </row>
+    <row r="61" spans="2:15">
+      <c r="E61" s="21"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="Q26:AK26"/>
-    <mergeCell ref="Q27:Q28"/>
-    <mergeCell ref="R27:AK27"/>
+    <mergeCell ref="Q27:AK27"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="R28:AK28"/>
   </mergeCells>
-  <conditionalFormatting sqref="R29:AK35">
+  <conditionalFormatting sqref="R30:AK36">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -4522,13 +3984,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B4:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
données à la main choix 7 à changer
</commit_message>
<xml_diff>
--- a/sprint_backlog.xlsx
+++ b/sprint_backlog.xlsx
@@ -20,12 +20,11 @@
     <definedName name="team_members">[1]Legend!$D$3:$D$9</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="86">
   <si>
     <t>N°</t>
   </si>
@@ -117,9 +116,6 @@
     <t>afficher le temps de parcours total</t>
   </si>
   <si>
-    <t>afficher les zones par lequelles l'utilisateur doit passer</t>
-  </si>
-  <si>
     <t>afficher les changements de lignes</t>
   </si>
   <si>
@@ -198,9 +194,6 @@
     <t>choisir des points de passage</t>
   </si>
   <si>
-    <t>définir les heures de passage d'une ligne</t>
-  </si>
-  <si>
     <t>afficher la station la plus proche par rapport à la destination</t>
   </si>
   <si>
@@ -265,6 +258,30 @@
   </si>
   <si>
     <t xml:space="preserve">architecture </t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>définir les lignes</t>
+  </si>
+  <si>
+    <t>affecter les perturbations sur les lignes</t>
+  </si>
+  <si>
+    <t>afficher le prochain passage d'une ligne à un arrêt</t>
+  </si>
+  <si>
+    <t>déterminer les terminus</t>
+  </si>
+  <si>
+    <t>gérer les aretes de retour</t>
+  </si>
+  <si>
+    <t>afficher les stations d'une ligne</t>
+  </si>
+  <si>
+    <t>définir les heures de passage d'une ligne(aller/retour)</t>
   </si>
 </sst>
 </file>
@@ -691,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -777,9 +794,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -789,6 +803,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -806,6 +824,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1182,7 +1204,7 @@
           <c:x val="0.11197945144513816"/>
           <c:y val="0.125"/>
           <c:w val="0.8385437991938256"/>
-          <c:h val="0.66500000000000203"/>
+          <c:h val="0.6650000000000027"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1210,8 +1232,8 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="50"/>
-        <c:axId val="59862400"/>
-        <c:axId val="59872384"/>
+        <c:axId val="72263936"/>
+        <c:axId val="72278016"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1239,7 +1261,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1269,18 +1291,18 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="59862400"/>
-        <c:axId val="59872384"/>
+        <c:axId val="72263936"/>
+        <c:axId val="72278016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59862400"/>
+        <c:axId val="72263936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1304,13 +1326,13 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59872384"/>
+        <c:crossAx val="72278016"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59872384"/>
+        <c:axId val="72278016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -1346,7 +1368,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59862400"/>
+        <c:crossAx val="72263936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1361,7 +1383,7 @@
           <c:x val="0.62500158946123618"/>
           <c:y val="2.5000000000000001E-2"/>
           <c:w val="0.17057198019351033"/>
-          <c:h val="0.1587754330708662"/>
+          <c:h val="0.15877543307086642"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1423,7 +1445,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1462,7 +1484,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1473,25 +1495,25 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:overlap val="100"/>
-        <c:axId val="59891712"/>
-        <c:axId val="59893248"/>
+        <c:axId val="71887488"/>
+        <c:axId val="72556928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59891712"/>
+        <c:axId val="71887488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59893248"/>
+        <c:crossAx val="72556928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59893248"/>
+        <c:axId val="72556928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,7 +1521,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59891712"/>
+        <c:crossAx val="71887488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1512,7 +1534,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2146,8 +2168,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B10:O53" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="B10:O53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B10:O55" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="B10:O55">
     <filterColumn colId="4"/>
     <filterColumn colId="6"/>
     <filterColumn colId="7"/>
@@ -2179,8 +2201,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="E55:J61" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="E55:J61"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="E56:J62" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="E56:J62"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Colonne1" dataDxfId="5"/>
     <tableColumn id="2" name="Colonne2" dataDxfId="4"/>
@@ -2496,10 +2518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:AK61"/>
+  <dimension ref="B3:AK62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2531,7 +2553,7 @@
     </row>
     <row r="6" spans="2:15">
       <c r="D6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="26">
         <v>40995</v>
@@ -2540,7 +2562,7 @@
     </row>
     <row r="7" spans="2:15">
       <c r="D7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="26">
         <v>41037</v>
@@ -2549,11 +2571,11 @@
     </row>
     <row r="8" spans="2:15" ht="18.75">
       <c r="D8" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="29">
         <f ca="1">DATEDIF(NOW(),E7,"D")</f>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -2577,31 +2599,31 @@
         <v>10</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="18.75" customHeight="1">
@@ -2612,34 +2634,34 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="H11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="J11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="L11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="N11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="12" spans="2:15">
@@ -2666,18 +2688,18 @@
       <c r="B13" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="47" t="s">
-        <v>63</v>
+      <c r="C13" s="46" t="s">
+        <v>61</v>
       </c>
       <c r="D13" s="35"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="49">
+      <c r="F13" s="48">
         <f>SUM(F14:F21)</f>
-        <v>6</v>
-      </c>
-      <c r="G13" s="50">
+        <v>5</v>
+      </c>
+      <c r="G13" s="49">
         <f>SUM(G14:G21)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -2693,17 +2715,17 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
         <v>4</v>
       </c>
       <c r="G14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -2716,25 +2738,15 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" s="43"/>
-      <c r="C15" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="46" t="s">
-        <v>40</v>
+      <c r="C15" s="42"/>
+      <c r="D15" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="E15" s="42"/>
-      <c r="F15" s="42">
-        <v>1</v>
-      </c>
-      <c r="G15" s="42">
-        <v>2</v>
-      </c>
-      <c r="H15" s="42">
-        <v>2</v>
-      </c>
-      <c r="I15" s="42">
-        <v>2</v>
-      </c>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="42"/>
       <c r="K15" s="42"/>
       <c r="L15" s="42"/>
@@ -2748,10 +2760,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
@@ -2775,10 +2787,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2798,10 +2810,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2821,10 +2833,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2844,10 +2856,10 @@
         <v>6</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2867,10 +2879,10 @@
         <v>7</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -2886,30 +2898,30 @@
     </row>
     <row r="22" spans="2:37">
       <c r="C22" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H22">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:37" s="36" customFormat="1" ht="18.75">
       <c r="B23" s="32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="46" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="35"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="49">
+      <c r="H23" s="48">
         <f>SUM(H24:H36,H14:H21)</f>
-        <v>31</v>
-      </c>
-      <c r="I23" s="50">
+        <v>29</v>
+      </c>
+      <c r="I23" s="49">
         <f>SUM(I24:I47,I14:I21)</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -2921,10 +2933,10 @@
     <row r="24" spans="2:37" s="37" customFormat="1" ht="18.75">
       <c r="B24" s="38"/>
       <c r="C24" s="39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="40"/>
       <c r="F24" s="40"/>
@@ -2945,10 +2957,10 @@
     <row r="25" spans="2:37" ht="18.75">
       <c r="B25" s="33"/>
       <c r="C25" s="34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1">
@@ -2969,10 +2981,10 @@
     <row r="26" spans="2:37">
       <c r="B26" s="7"/>
       <c r="C26" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1">
@@ -2997,10 +3009,10 @@
     <row r="27" spans="2:37" ht="23.25">
       <c r="B27" s="42"/>
       <c r="C27" s="42" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -3017,37 +3029,37 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="Q27" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="R27" s="51"/>
-      <c r="S27" s="51"/>
-      <c r="T27" s="51"/>
-      <c r="U27" s="51"/>
-      <c r="V27" s="51"/>
-      <c r="W27" s="51"/>
-      <c r="X27" s="51"/>
-      <c r="Y27" s="51"/>
-      <c r="Z27" s="51"/>
-      <c r="AA27" s="51"/>
-      <c r="AB27" s="51"/>
-      <c r="AC27" s="51"/>
-      <c r="AD27" s="51"/>
-      <c r="AE27" s="51"/>
-      <c r="AF27" s="51"/>
-      <c r="AG27" s="51"/>
-      <c r="AH27" s="51"/>
-      <c r="AI27" s="51"/>
-      <c r="AJ27" s="51"/>
-      <c r="AK27" s="51"/>
+      <c r="Q27" s="52" t="s">
+        <v>41</v>
+      </c>
+      <c r="R27" s="52"/>
+      <c r="S27" s="52"/>
+      <c r="T27" s="52"/>
+      <c r="U27" s="52"/>
+      <c r="V27" s="52"/>
+      <c r="W27" s="52"/>
+      <c r="X27" s="52"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="52"/>
+      <c r="AA27" s="52"/>
+      <c r="AB27" s="52"/>
+      <c r="AC27" s="52"/>
+      <c r="AD27" s="52"/>
+      <c r="AE27" s="52"/>
+      <c r="AF27" s="52"/>
+      <c r="AG27" s="52"/>
+      <c r="AH27" s="52"/>
+      <c r="AI27" s="52"/>
+      <c r="AJ27" s="52"/>
+      <c r="AK27" s="52"/>
     </row>
     <row r="28" spans="2:37">
       <c r="B28" s="42"/>
       <c r="C28" s="42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -3064,39 +3076,39 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="Q28" s="52" t="s">
-        <v>41</v>
-      </c>
-      <c r="R28" s="54" t="s">
-        <v>43</v>
-      </c>
-      <c r="S28" s="55"/>
-      <c r="T28" s="55"/>
-      <c r="U28" s="55"/>
-      <c r="V28" s="55"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="55"/>
-      <c r="Y28" s="55"/>
-      <c r="Z28" s="55"/>
-      <c r="AA28" s="55"/>
-      <c r="AB28" s="55"/>
-      <c r="AC28" s="55"/>
-      <c r="AD28" s="55"/>
-      <c r="AE28" s="55"/>
-      <c r="AF28" s="55"/>
-      <c r="AG28" s="55"/>
-      <c r="AH28" s="55"/>
-      <c r="AI28" s="55"/>
-      <c r="AJ28" s="55"/>
-      <c r="AK28" s="56"/>
+      <c r="Q28" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="R28" s="55" t="s">
+        <v>42</v>
+      </c>
+      <c r="S28" s="56"/>
+      <c r="T28" s="56"/>
+      <c r="U28" s="56"/>
+      <c r="V28" s="56"/>
+      <c r="W28" s="56"/>
+      <c r="X28" s="56"/>
+      <c r="Y28" s="56"/>
+      <c r="Z28" s="56"/>
+      <c r="AA28" s="56"/>
+      <c r="AB28" s="56"/>
+      <c r="AC28" s="56"/>
+      <c r="AD28" s="56"/>
+      <c r="AE28" s="56"/>
+      <c r="AF28" s="56"/>
+      <c r="AG28" s="56"/>
+      <c r="AH28" s="56"/>
+      <c r="AI28" s="56"/>
+      <c r="AJ28" s="56"/>
+      <c r="AK28" s="57"/>
     </row>
     <row r="29" spans="2:37">
       <c r="B29" s="43"/>
       <c r="C29" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="46" t="s">
-        <v>40</v>
+      <c r="D29" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -3113,7 +3125,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
-      <c r="Q29" s="53"/>
+      <c r="Q29" s="54"/>
       <c r="R29" s="9">
         <v>1</v>
       </c>
@@ -3208,10 +3220,10 @@
     <row r="31" spans="2:37">
       <c r="B31" s="43"/>
       <c r="C31" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="44" t="s">
-        <v>22</v>
+        <v>56</v>
+      </c>
+      <c r="D31" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -3219,7 +3231,9 @@
       <c r="H31" s="1">
         <v>3</v>
       </c>
-      <c r="I31" s="1"/>
+      <c r="I31" s="1">
+        <v>3</v>
+      </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -3270,8 +3284,8 @@
       <c r="C32" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="45" t="s">
-        <v>4</v>
+      <c r="D32" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -3280,7 +3294,7 @@
         <v>2</v>
       </c>
       <c r="I32" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -3332,8 +3346,8 @@
       <c r="C33" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="45" t="s">
-        <v>4</v>
+      <c r="D33" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -3390,10 +3404,10 @@
     <row r="34" spans="2:37">
       <c r="B34" s="43"/>
       <c r="C34" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="46" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="D34" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -3452,8 +3466,8 @@
       <c r="C35" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="46" t="s">
-        <v>40</v>
+      <c r="D35" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -3510,10 +3524,10 @@
     <row r="36" spans="2:37">
       <c r="B36" s="43"/>
       <c r="C36" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="46" t="s">
         <v>67</v>
+      </c>
+      <c r="D36" s="45" t="s">
+        <v>65</v>
       </c>
       <c r="E36" s="42"/>
       <c r="F36" s="42"/>
@@ -3572,8 +3586,8 @@
       <c r="C37" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="46" t="s">
-        <v>40</v>
+      <c r="D37" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="E37" s="42"/>
       <c r="F37" s="42"/>
@@ -3594,7 +3608,7 @@
     <row r="38" spans="2:37">
       <c r="B38" s="42"/>
       <c r="C38" s="42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D38" s="42"/>
       <c r="E38" s="42"/>
@@ -3611,12 +3625,15 @@
     </row>
     <row r="39" spans="2:37">
       <c r="C39" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="2:37" s="36" customFormat="1" ht="18.75">
       <c r="B40" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>17</v>
@@ -3627,10 +3644,10 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="48">
+      <c r="J40" s="47">
         <v>5</v>
       </c>
-      <c r="K40" s="48"/>
+      <c r="K40" s="47"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
@@ -3639,10 +3656,10 @@
     <row r="41" spans="2:37">
       <c r="B41" s="43"/>
       <c r="C41" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="D41" s="44" t="s">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="D41" s="50" t="s">
+        <v>4</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -3652,7 +3669,9 @@
       <c r="J41" s="1">
         <v>3</v>
       </c>
-      <c r="K41" s="1"/>
+      <c r="K41" s="1">
+        <v>3</v>
+      </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
@@ -3661,10 +3680,10 @@
     <row r="42" spans="2:37">
       <c r="B42" s="43"/>
       <c r="C42" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="44" t="s">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -3672,9 +3691,11 @@
       <c r="H42" s="42"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1">
-        <v>3</v>
-      </c>
-      <c r="K42" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="K42" s="1">
+        <v>4</v>
+      </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
@@ -3683,7 +3704,7 @@
     <row r="43" spans="2:37">
       <c r="B43" s="43"/>
       <c r="C43" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D43" s="44" t="s">
         <v>22</v>
@@ -3705,10 +3726,10 @@
     <row r="44" spans="2:37">
       <c r="B44" s="7"/>
       <c r="C44" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="D44" s="44" t="s">
-        <v>22</v>
+        <v>85</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -3716,9 +3737,11 @@
       <c r="H44" s="42"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1">
-        <v>1</v>
-      </c>
-      <c r="K44" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="K44" s="1">
+        <v>3</v>
+      </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
@@ -3729,8 +3752,8 @@
       <c r="C45" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D45" s="46" t="s">
-        <v>40</v>
+      <c r="D45" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -3740,7 +3763,9 @@
       <c r="J45" s="1">
         <v>2</v>
       </c>
-      <c r="K45" s="1"/>
+      <c r="K45" s="1">
+        <v>1</v>
+      </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
@@ -3749,18 +3774,22 @@
     <row r="46" spans="2:37">
       <c r="B46" s="43"/>
       <c r="C46" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" s="44" t="s">
-        <v>22</v>
+        <v>83</v>
+      </c>
+      <c r="D46" s="45" t="s">
+        <v>39</v>
       </c>
       <c r="E46" s="42"/>
       <c r="F46" s="42"/>
       <c r="G46" s="42"/>
       <c r="H46" s="42"/>
       <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="1"/>
+      <c r="J46" s="42">
+        <v>2</v>
+      </c>
+      <c r="K46" s="1">
+        <v>2</v>
+      </c>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
@@ -3769,18 +3798,22 @@
     <row r="47" spans="2:37">
       <c r="B47" s="43"/>
       <c r="C47" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="D47" s="44" t="s">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="D47" s="50" t="s">
+        <v>4</v>
       </c>
       <c r="E47" s="42"/>
       <c r="F47" s="42"/>
       <c r="G47" s="42"/>
       <c r="H47" s="42"/>
       <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
-      <c r="K47" s="1"/>
+      <c r="J47" s="42">
+        <v>3</v>
+      </c>
+      <c r="K47" s="1">
+        <v>3</v>
+      </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
@@ -3789,27 +3822,39 @@
     <row r="48" spans="2:37">
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D48" s="42"/>
+        <v>69</v>
+      </c>
+      <c r="D48" s="50" t="s">
+        <v>4</v>
+      </c>
       <c r="E48" s="42"/>
       <c r="F48" s="42"/>
       <c r="G48" s="42"/>
       <c r="H48" s="42"/>
       <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
+      <c r="J48" s="42">
+        <v>3</v>
+      </c>
+      <c r="K48" s="1">
+        <v>3</v>
+      </c>
+      <c r="L48" s="1">
+        <v>2</v>
+      </c>
+      <c r="M48" s="1">
+        <v>1</v>
+      </c>
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
     </row>
     <row r="49" spans="2:15">
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D49" s="42"/>
+        <v>70</v>
+      </c>
+      <c r="D49" s="44" t="s">
+        <v>22</v>
+      </c>
       <c r="E49" s="42"/>
       <c r="F49" s="42"/>
       <c r="G49" s="42"/>
@@ -3823,32 +3868,48 @@
       <c r="O49" s="1"/>
     </row>
     <row r="50" spans="2:15">
-      <c r="B50" s="1"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="45" t="s">
+        <v>39</v>
+      </c>
       <c r="E50" s="42"/>
       <c r="F50" s="42"/>
       <c r="G50" s="42"/>
       <c r="H50" s="42"/>
       <c r="I50" s="42"/>
-      <c r="J50" s="42"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
+      <c r="J50" s="42">
+        <v>3</v>
+      </c>
+      <c r="K50" s="42">
+        <v>3</v>
+      </c>
+      <c r="L50" s="42"/>
+      <c r="M50" s="42"/>
+      <c r="N50" s="42"/>
+      <c r="O50" s="42"/>
     </row>
     <row r="51" spans="2:15">
       <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="42">
+        <v>2</v>
+      </c>
+      <c r="K51" s="1">
+        <v>2</v>
+      </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
@@ -3856,82 +3917,156 @@
     </row>
     <row r="52" spans="2:15">
       <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
+      <c r="C52" t="s">
+        <v>77</v>
+      </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
+      <c r="J52" s="1">
+        <v>3</v>
+      </c>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="2:15">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-    </row>
-    <row r="55" spans="2:15" hidden="1">
-      <c r="E55" t="s">
+    <row r="53" spans="2:15" s="36" customFormat="1" ht="18.75">
+      <c r="B53" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="35"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="47">
         <v>5</v>
       </c>
-      <c r="F55" t="s">
+      <c r="K53" s="47"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+      <c r="O53" s="2"/>
+    </row>
+    <row r="54" spans="2:15">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1">
+        <v>2</v>
+      </c>
+      <c r="M54" s="1">
+        <v>2</v>
+      </c>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+    </row>
+    <row r="55" spans="2:15">
+      <c r="B55" s="51"/>
+      <c r="C55" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="51"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="51"/>
+      <c r="J55" s="51"/>
+      <c r="K55" s="51"/>
+      <c r="L55" s="51">
+        <v>4</v>
+      </c>
+      <c r="M55" s="51">
+        <v>4</v>
+      </c>
+      <c r="N55" s="51"/>
+      <c r="O55" s="51"/>
+    </row>
+    <row r="56" spans="2:15" hidden="1">
+      <c r="E56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F56" t="s">
         <v>6</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G56" t="s">
         <v>7</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H56" t="s">
         <v>8</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I56" t="s">
         <v>9</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J56" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="2:15" ht="15.75">
-      <c r="E56" s="19"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-    </row>
-    <row r="57" spans="2:15">
-      <c r="E57" s="20"/>
+    <row r="57" spans="2:15" ht="15.75">
+      <c r="C57" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="19"/>
       <c r="F57" s="20"/>
       <c r="G57" s="20"/>
       <c r="H57" s="20"/>
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="2:15">
+      <c r="C58" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="59" t="s">
+        <v>39</v>
+      </c>
       <c r="E58" s="20"/>
       <c r="F58" s="20"/>
       <c r="G58" s="20"/>
       <c r="H58" s="20"/>
       <c r="I58" s="20"/>
       <c r="J58" s="20"/>
+      <c r="L58">
+        <v>2</v>
+      </c>
+      <c r="M58">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="2:15">
-      <c r="E59" s="21"/>
+      <c r="E59" s="20"/>
       <c r="F59" s="20"/>
       <c r="G59" s="20"/>
       <c r="H59" s="20"/>
@@ -3953,6 +4088,14 @@
       <c r="H61" s="20"/>
       <c r="I61" s="20"/>
       <c r="J61" s="20"/>
+    </row>
+    <row r="62" spans="2:15">
+      <c r="E62" s="21"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4005,47 +4148,47 @@
   <sheetData>
     <row r="4" spans="2:10">
       <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
         <v>73</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" t="s">
-        <v>75</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:10">
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s">
         <v>75</v>
-      </c>
-      <c r="H5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:10">
       <c r="B7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>